<commit_message>
Fix one sample ids in the lookup table
</commit_message>
<xml_diff>
--- a/Sample_ID_Lookup_table_in_repositories.xlsx
+++ b/Sample_ID_Lookup_table_in_repositories.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/allakarpova/Box Sync/snATAC_pancan/tumor_Alla/Suppl.tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nadezhdaterekhanova/Desktop/Git_hub/Public_dirs/PanCan_snATAC_publication/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E7E1F5-B734-F344-904D-E6DD6B94BBDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E275DAD9-757F-C44E-BB53-9BC62D58DFDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1240" yWindow="500" windowWidth="34600" windowHeight="21900" activeTab="1" xr2:uid="{8A857C8D-A7ED-5E4A-9723-60A27A53F0CD}"/>
+    <workbookView xWindow="36940" yWindow="3900" windowWidth="30340" windowHeight="19620" activeTab="1" xr2:uid="{8A857C8D-A7ED-5E4A-9723-60A27A53F0CD}"/>
   </bookViews>
   <sheets>
     <sheet name="ATAC data" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3926" uniqueCount="760">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3926" uniqueCount="763">
   <si>
     <t>BM2</t>
   </si>
@@ -2317,6 +2317,15 @@
   </si>
   <si>
     <t>https://portal.gdc.cancer.gov/</t>
+  </si>
+  <si>
+    <t>HTA12_28</t>
+  </si>
+  <si>
+    <t>HTA12_28_4</t>
+  </si>
+  <si>
+    <t>HTA12_28_6</t>
   </si>
 </sst>
 </file>
@@ -2469,7 +2478,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2495,7 +2504,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -13774,8 +13782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FE89A45-DC42-6348-9E61-BFC731B13A17}">
   <dimension ref="A1:M1027"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="H123" sqref="H123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14673,7 +14681,7 @@
       <c r="D32" s="1" t="s">
         <v>692</v>
       </c>
-      <c r="E32" s="21" t="s">
+      <c r="E32" t="s">
         <v>744</v>
       </c>
       <c r="F32" s="8" t="s">
@@ -14855,7 +14863,7 @@
       <c r="D38" s="1" t="s">
         <v>692</v>
       </c>
-      <c r="E38" s="21" t="s">
+      <c r="E38" t="s">
         <v>745</v>
       </c>
       <c r="F38" s="8" t="s">
@@ -15037,7 +15045,7 @@
       <c r="D44" s="1" t="s">
         <v>692</v>
       </c>
-      <c r="E44" s="21" t="s">
+      <c r="E44" t="s">
         <v>746</v>
       </c>
       <c r="F44" s="8" t="s">
@@ -15099,7 +15107,7 @@
       <c r="D46" s="1" t="s">
         <v>692</v>
       </c>
-      <c r="E46" s="21" t="s">
+      <c r="E46" t="s">
         <v>747</v>
       </c>
       <c r="F46" s="8" t="s">
@@ -15131,7 +15139,7 @@
       <c r="D47" s="1" t="s">
         <v>692</v>
       </c>
-      <c r="E47" s="21" t="s">
+      <c r="E47" t="s">
         <v>748</v>
       </c>
       <c r="F47" s="8" t="s">
@@ -15163,7 +15171,7 @@
       <c r="D48" s="1" t="s">
         <v>692</v>
       </c>
-      <c r="E48" s="21" t="s">
+      <c r="E48" t="s">
         <v>749</v>
       </c>
       <c r="F48" s="8" t="s">
@@ -15225,7 +15233,7 @@
       <c r="D50" s="1" t="s">
         <v>692</v>
       </c>
-      <c r="E50" s="21" t="s">
+      <c r="E50" t="s">
         <v>750</v>
       </c>
       <c r="F50" s="8" t="s">
@@ -15287,7 +15295,7 @@
       <c r="D52" s="1" t="s">
         <v>692</v>
       </c>
-      <c r="E52" s="21" t="s">
+      <c r="E52" t="s">
         <v>751</v>
       </c>
       <c r="F52" s="8" t="s">
@@ -15319,7 +15327,7 @@
       <c r="D53" s="1" t="s">
         <v>692</v>
       </c>
-      <c r="E53" s="21" t="s">
+      <c r="E53" t="s">
         <v>752</v>
       </c>
       <c r="F53" s="8" t="s">
@@ -15351,7 +15359,7 @@
       <c r="D54" s="1" t="s">
         <v>692</v>
       </c>
-      <c r="E54" s="21" t="s">
+      <c r="E54" t="s">
         <v>753</v>
       </c>
       <c r="F54" s="8" t="s">
@@ -15383,7 +15391,7 @@
       <c r="D55" s="1" t="s">
         <v>692</v>
       </c>
-      <c r="E55" s="21" t="s">
+      <c r="E55" t="s">
         <v>754</v>
       </c>
       <c r="F55" s="8" t="s">
@@ -15415,7 +15423,7 @@
       <c r="D56" s="1" t="s">
         <v>692</v>
       </c>
-      <c r="E56" s="21" t="s">
+      <c r="E56" t="s">
         <v>755</v>
       </c>
       <c r="F56" s="8" t="s">
@@ -17469,10 +17477,10 @@
         <v>588</v>
       </c>
       <c r="G122" s="8" t="s">
-        <v>385</v>
+        <v>760</v>
       </c>
       <c r="H122" s="8" t="s">
-        <v>386</v>
+        <v>761</v>
       </c>
       <c r="I122" s="8" t="s">
         <v>574</v>
@@ -17500,10 +17508,10 @@
         <v>588</v>
       </c>
       <c r="G123" s="8" t="s">
-        <v>385</v>
+        <v>760</v>
       </c>
       <c r="H123" s="8" t="s">
-        <v>387</v>
+        <v>762</v>
       </c>
       <c r="I123" s="8" t="s">
         <v>574</v>

</xml_diff>